<commit_message>
Decrease the increase of required XP per level by 33%
</commit_message>
<xml_diff>
--- a/dist/n4bb12_XPPlayerProgression/progression.xlsx
+++ b/dist/n4bb12_XPPlayerProgression/progression.xlsx
@@ -182,10 +182,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Chart!$D$2:$D$100</c:f>
+              <c:f>Chart!$D$2:$D$300</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="99"/>
+                <c:ptCount val="299"/>
                 <c:pt idx="0">
                   <c:v>9831.560085449999</c:v>
                 </c:pt>
@@ -482,6 +482,606 @@
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>41889.114851965758</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>42513.262663260051</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>43146.71027694262</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>43789.596260069062</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>44442.061244344099</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>45104.247956884814</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>45776.301251442404</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>46458.368140088889</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>47150.597825376222</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>47853.14173297432</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>48566.153544795634</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>49289.789232613097</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>50024.207092179029</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>50769.567777852484</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>51526.034337742494</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>52293.772249374859</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>53072.949455890557</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>53863.73640278331</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>54666.306075184773</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>55480.834035705026</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>56307.498462837044</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>57146.480189933296</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>57997.962744763303</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>58862.132389660284</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>59739.178162266217</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>60629.291916883994</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>61532.668366445549</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>62449.505125105592</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>63380.00275146967</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>64324.364792466557</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>65282.797827874318</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>66255.511515509628</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>67242.718637090729</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>68244.635144783388</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>69261.480208440655</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>70293.476263546414</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>71340.849059873261</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>72403.827710865356</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>73482.644743757264</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>74577.536150439249</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>75688.741439080783</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>76816.503686523094</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>77961.06959145228</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>79122.689528364906</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>80301.617602337559</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>81498.111704612369</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>82712.433569011104</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>83944.848829189359</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>85195.627076744291</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>86465.041920187767</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>87753.37104479858</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>89060.896273366059</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>90387.90362783923</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>91734.68339189401</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>93101.530174433239</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>94488.742974032313</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>95896.625244345385</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>97325.484960486123</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>98775.634686397345</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>100247.39164322466</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>101741.07777870874</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>103257.01983761147</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>104795.5494331919</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>106357.00311974646</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>107941.72246623067</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>109550.05413097751</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>111182.34993752906</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>112838.96695159824</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>114520.26755917707</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>116226.61954580878</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>117958.39617704134</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>119715.97628007927</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>121499.74432665245</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>123310.09051711955</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>125147.41086582461</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>127012.10728772543</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>128904.58768631253</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>130825.26604283856</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>132774.56250687686</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>134752.90348822935</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>136760.72175020399</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>138798.45650428199</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>140866.55350619578</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>142965.4651534381</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>145095.65058422432</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>147257.57577792922</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>149451.71365702039</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>151678.54419051</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>153938.55449894862</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>156232.23896098297</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>158560.09932150159</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>160922.64480139196</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>163320.3922089327</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>165753.86605284575</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>168223.59865703314</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>170730.13027702298</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>173274.00921815063</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>175855.79195550104</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>178476.04325563801</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>181135.33630014703</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>183834.25281101922</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>186573.38317790336</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>189353.32658725415</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>192174.69115340424</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>195038.09405158996</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>197944.16165295863</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>200893.5296615877</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>203886.84325354538</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>206924.75721802318</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>210007.93610057171</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>213137.05434847024</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>216312.79645826243</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>219535.85712549058</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>222806.94139666038</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>226126.76482347058</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>229496.05361934027</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>232915.54481826845</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>236385.9864360606</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>239908.13763395796</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>243482.76888470398</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>247110.66214108601</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>250792.61100698821</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>254529.42091099228</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>258321.90928256608</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>262170.90573087631</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>266077.25222626637</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>270041.80328443774</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>274065.42615337588</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>278149.00100306119</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>282293.42111800675</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>286499.59309266508</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>290768.43702974572</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>295100.886741489</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>299497.88995393709</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>303960.40851425083</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>308489.41860111314</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>313085.91093826969</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>317750.89101124991</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>322485.37928731751</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>327290.41143869859</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>332167.03856913513</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>337116.32744381524</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>342139.36072272813</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>347237.23719749675</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>352411.07203173952</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>357661.99700501229</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>362991.16076038696</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>368399.72905571677</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>373888.88501864701</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>379459.82940542471</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>385113.78086356557</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>390851.97619843273</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>396675.6706437894</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>402586.13813638192</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>408584.67159461393</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>414672.58320137364</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>420851.20469107415</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>427121.88764097117</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>433486.00376682164</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>439944.94522294722</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>446500.1249067692</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>453152.97676788003</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>459904.95612172136</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>466757.53996793501</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>473712.22731345729</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>480770.53950042772</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>487934.0205389841</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>495204.23744501499</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>502582.78058294574</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>510071.26401363156</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>517671.32584743469</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>525384.62860256142</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>533212.85956873966</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>541157.73117631371</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>549220.9813708408</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>557404.37399326637</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>565709.69916576613</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>574138.77368333586</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>582693.44141121767</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>591375.57368824468</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>600187.06973619957</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>609129.85707526887</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>618205.89194569038</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>627417.15973568137</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>636765.67541574291</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>646253.4839794375</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>655882.66089073091</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>665655.31253800285</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>675573.57669481914</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>685639.62298757187</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>695855.6533700868</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>706223.902605301</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>716746.6387541201</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>727426.16367155639</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>738264.81351026252</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>749264.95923156536</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>760429.00712411571</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>771759.39933026489</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>783258.61438028596</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>794929.16773455229</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>806773.61233379715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,10 +1096,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Chart!$I$2:$I$100</c:f>
+              <c:f>Chart!$I$2:$I$300</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="99"/>
+                <c:ptCount val="299"/>
                 <c:pt idx="0">
                   <c:v>10201</c:v>
                 </c:pt>
@@ -796,6 +1396,606 @@
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>27048.138294215289</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>27318.619677157443</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>27591.805873929021</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>27867.723932668301</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>28146.401171994992</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>28427.865183714945</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>28712.143835552099</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>28999.265273907611</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>29289.257926646689</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>29582.15050591316</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>29877.972010972295</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>30176.751731082008</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>30478.519248392833</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>30783.304440876767</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>31091.137485285537</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>31402.048860138384</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>31716.069348739769</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>32033.230042227166</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>32353.562342649446</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>32677.097966075933</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>33003.8689457367</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>33333.907635194068</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>33667.246711546009</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>34003.919178661461</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>34343.958370448076</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>34687.397954152562</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>35034.271933694094</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>35384.614653031022</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>35738.460799561341</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>36095.845407556953</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>36456.803861632521</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>36821.371900248843</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>37189.585619251338</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>37561.481475443841</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>37937.096290198286</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>38316.467253100265</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>38699.631925631278</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>39086.628244887594</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>39477.494527336472</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>39872.269472609827</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>40270.992167335928</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>40673.70208900929</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>41080.43910989938</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>41491.243500998367</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>41906.155936008363</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>42325.217495368452</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>42748.469670322134</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43175.954367025348</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43607.713910695602</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>44043.791049802552</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>44484.228960300592</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>44929.071249903594</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>45378.361962402632</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>45832.145582026671</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>46290.467037846931</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>46753.371708225393</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>47220.905425307639</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>47693.114479560725</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>48170.045624356339</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>48651.746080599885</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>49138.263541405897</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>49629.646176819959</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>50125.94263858816</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>50627.20206497403</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>51133.474085623777</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>51644.808826480017</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>52161.256914744823</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>52682.869483892253</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>53209.698178731196</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>53741.795160518508</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>54279.213112123703</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>54822.005243244923</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>55370.225295677374</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>55923.92754863415</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>56483.166824120497</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>57047.998492361679</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>57618.478477285324</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>58194.663262058173</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>58776.609894678761</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>59364.375993625537</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>59958.019753561799</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>60557.599951097407</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>61163.175950608391</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>61774.807710114466</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>62392.555787215628</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>63016.481345087792</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>63646.646158538671</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>64283.112620124033</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>64925.943746325283</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>65575.20318378853</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>66230.955215626425</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>66893.264767782675</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>67562.197415460512</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>68237.819389615121</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>68920.197583511283</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>69609.399559346377</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>70305.493554939851</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>71008.548490489251</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>71718.633975394157</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>72435.82031514807</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>73160.178518299566</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>73891.780303482563</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>74630.69810651739</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>75377.005087582555</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>76130.775138458383</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>76892.082889842961</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>77661.003718741413</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>78437.613755928804</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>79221.98989348812</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>80014.209792422989</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>80814.351890347243</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>81622.495409250696</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>82438.720363343222</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>83263.107566976629</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>84095.738642646422</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>84936.69602907286</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>85786.062989363607</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>86643.923619257257</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>87510.362855449843</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>88385.466484004311</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>89269.321148844348</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>90162.014360332789</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>91063.634503936133</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>91974.270848975473</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>92894.013557465252</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>93822.953693039904</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>94761.183229970295</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>95708.795062270001</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>96665.883012892693</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>97632.541843021623</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>98608.867261451858</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>99594.95593406634</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>100590.90549340704</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>101596.81454834111</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>102612.78269382456</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>103638.91052076274</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>104675.29962597039</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>105722.05262223011</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>106779.27314845241</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>107847.06587993691</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>108925.5365387363</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>110014.79190412369</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>111114.93982316492</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>112226.08922139654</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>113348.35011361052</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>114481.83361474662</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>115626.65195089413</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>116782.91847040302</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>117950.74765510709</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>119130.25513165817</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>120321.55768297473</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>121524.77325980445</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>122740.02099240251</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>123967.42120232654</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>125207.09541434982</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>126459.16636849329</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>127723.75803217824</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>129000.99561250003</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>130291.00556862503</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>131593.91562431128</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>132909.85478055439</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>134238.95332835993</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>135581.34286164356</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>136937.15629025994</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>138306.52785316258</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>139689.59313169422</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>141086.48906301116</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>142497.35395364126</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>143922.32749317767</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>145361.55076810945</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>146815.16627579057</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>148283.31793854843</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>149766.15111793397</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>151263.81262911329</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>152776.45075540445</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>154304.21526295846</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>155847.25741558807</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>157405.72998974391</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>158979.78728964139</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>160569.58516253778</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>162175.28101416319</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>163797.03382430485</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>165435.00416254791</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>167089.35420417335</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>168760.24774621506</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>170447.85022367723</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>172152.32872591403</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>173873.85201317311</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>175612.59053330487</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>177368.71643863793</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>179142.40360302432</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>180933.82763905454</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>182743.16591544508</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>184570.59757459955</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>186416.30355034556</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>188280.46658584895</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>190163.27125170751</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>192064.90396422459</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>193985.55300386687</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>195925.40853390549</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>197884.66261924454</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,11 +2012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="214850560"/>
-        <c:axId val="214860544"/>
+        <c:axId val="189082624"/>
+        <c:axId val="213742336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="214850560"/>
+        <c:axId val="189082624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +2025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214860544"/>
+        <c:crossAx val="213742336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -833,7 +2033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214860544"/>
+        <c:axId val="213742336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,7 +2044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214850560"/>
+        <c:crossAx val="189082624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1190,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>